<commit_message>
Review Progress & New Course Items
Reviewing all the progress so far and trying the warm up exercise in Milestone Project 2
</commit_message>
<xml_diff>
--- a/1.Course/0.Extras/Complete_Python_Bootcamp_Zero_To_Hero.xlsx
+++ b/1.Course/0.Extras/Complete_Python_Bootcamp_Zero_To_Hero.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="312">
   <si>
     <t>Introduction</t>
   </si>
@@ -331,13 +331,634 @@
   </si>
   <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>–Course Overview</t>
+  </si>
+  <si>
+    <t>Auto-Welcome Message </t>
+  </si>
+  <si>
+    <t>Course Introduction </t>
+  </si>
+  <si>
+    <t>Preview06:39</t>
+  </si>
+  <si>
+    <t>Course Curriculum Overview </t>
+  </si>
+  <si>
+    <t>Why Python? </t>
+  </si>
+  <si>
+    <t>Course FAQs </t>
+  </si>
+  <si>
+    <t>–Python Setup</t>
+  </si>
+  <si>
+    <t>Command Line Basics </t>
+  </si>
+  <si>
+    <t>Installing Python (Step by Step) </t>
+  </si>
+  <si>
+    <t>Preview08:18</t>
+  </si>
+  <si>
+    <t>Running Python Code </t>
+  </si>
+  <si>
+    <t>Getting the Notebooks and the Course Material </t>
+  </si>
+  <si>
+    <t>Git and Github Overview (Optional) </t>
+  </si>
+  <si>
+    <t>–Python Object and Data Structure Basics</t>
+  </si>
+  <si>
+    <t>Introduction to Python Data Types </t>
+  </si>
+  <si>
+    <t>Python Numbers </t>
+  </si>
+  <si>
+    <t>Preview04:11</t>
+  </si>
+  <si>
+    <t>Numbers: Simple Arithmetic</t>
+  </si>
+  <si>
+    <t>1 question</t>
+  </si>
+  <si>
+    <t>Numbers - FAQ </t>
+  </si>
+  <si>
+    <t>Numbers Quiz </t>
+  </si>
+  <si>
+    <t>3 questions</t>
+  </si>
+  <si>
+    <t>Variable Assignments </t>
+  </si>
+  <si>
+    <t>Introduction to Strings </t>
+  </si>
+  <si>
+    <t>Quick Print Check</t>
+  </si>
+  <si>
+    <t>Indexing and Slicing with Strings </t>
+  </si>
+  <si>
+    <t>String Indexing</t>
+  </si>
+  <si>
+    <t>String Slicing</t>
+  </si>
+  <si>
+    <t>String Properties and Methods </t>
+  </si>
+  <si>
+    <t>Strings -FAQ </t>
+  </si>
+  <si>
+    <t>Strings Quiz</t>
+  </si>
+  <si>
+    <t>Print Formatting with Strings </t>
+  </si>
+  <si>
+    <t>Print Formatting FAQs </t>
+  </si>
+  <si>
+    <t>Print Formatting</t>
+  </si>
+  <si>
+    <t>Lists in Python </t>
+  </si>
+  <si>
+    <t>Lists - FAQ </t>
+  </si>
+  <si>
+    <t>Lists Quiz</t>
+  </si>
+  <si>
+    <t>Dictionaries in Python </t>
+  </si>
+  <si>
+    <t>Dictionaries - FAQ </t>
+  </si>
+  <si>
+    <t>Dictionaries Quiz</t>
+  </si>
+  <si>
+    <t>Tuples with Python </t>
+  </si>
+  <si>
+    <t>Tuples Quiz</t>
+  </si>
+  <si>
+    <t>Sets in Python </t>
+  </si>
+  <si>
+    <t>Booleans in Python </t>
+  </si>
+  <si>
+    <t>Sets and Booleans Quiz</t>
+  </si>
+  <si>
+    <t>I/O with Basic Files in Python </t>
+  </si>
+  <si>
+    <t>File I/O</t>
+  </si>
+  <si>
+    <t>Resources for More Basic Practice </t>
+  </si>
+  <si>
+    <t>Python Objects and Data Structures Assessment Test Overview </t>
+  </si>
+  <si>
+    <t>Python Objects and Data Structures Assessment Test Solutions </t>
+  </si>
+  <si>
+    <t>–Python Comparison Operators</t>
+  </si>
+  <si>
+    <t>Comparison Operators in Python </t>
+  </si>
+  <si>
+    <t>Chaining Comparison Operators in Python with Logical Operators </t>
+  </si>
+  <si>
+    <t>Comparison Operators Quiz </t>
+  </si>
+  <si>
+    <t>5 questions</t>
+  </si>
+  <si>
+    <t>–Python Statements</t>
+  </si>
+  <si>
+    <t>If Elif and Else Statements in Python </t>
+  </si>
+  <si>
+    <t>For Loops in Python </t>
+  </si>
+  <si>
+    <t>Preview18:17</t>
+  </si>
+  <si>
+    <t>While Loops in Python </t>
+  </si>
+  <si>
+    <t>Useful Operators in Python </t>
+  </si>
+  <si>
+    <t>List Comprehensions in Python </t>
+  </si>
+  <si>
+    <t>Python Statements Test Overview </t>
+  </si>
+  <si>
+    <t>Python Statements Test Solutions </t>
+  </si>
+  <si>
+    <t>–Methods and Functions</t>
+  </si>
+  <si>
+    <t>Methods and the Python Documentation </t>
+  </si>
+  <si>
+    <t>Introduction to Functions </t>
+  </si>
+  <si>
+    <t>def Keyword </t>
+  </si>
+  <si>
+    <t>Basics of Python Functions </t>
+  </si>
+  <si>
+    <t>Logic with Python Functions </t>
+  </si>
+  <si>
+    <t>Tuple Unpacking with Python Functions </t>
+  </si>
+  <si>
+    <t>Interactions between Python Functions </t>
+  </si>
+  <si>
+    <t>Overview of Quick Function Exercises #1-10 </t>
+  </si>
+  <si>
+    <t>Quick Check on Solutions Link </t>
+  </si>
+  <si>
+    <t>Functions #1: print Hello World</t>
+  </si>
+  <si>
+    <t>Functions #2: print Hello Name</t>
+  </si>
+  <si>
+    <t>Functions #3 - simple Boolean</t>
+  </si>
+  <si>
+    <t>Functions #4 - using Booleans</t>
+  </si>
+  <si>
+    <t>Functions #5: simple math</t>
+  </si>
+  <si>
+    <t>Functions #6: is even</t>
+  </si>
+  <si>
+    <t>Functions #7: is greater</t>
+  </si>
+  <si>
+    <t>*args and **kwargs in Python </t>
+  </si>
+  <si>
+    <t>Functions #8: *args</t>
+  </si>
+  <si>
+    <t>Functions #9: pick evens</t>
+  </si>
+  <si>
+    <t>Functions #10: skyline</t>
+  </si>
+  <si>
+    <t>Function Practice Exercises - Overview </t>
+  </si>
+  <si>
+    <t>Function Practice Exercises - Solutions </t>
+  </si>
+  <si>
+    <t>Function Practice - Solutions Level One </t>
+  </si>
+  <si>
+    <t>Function Practice - Solutions Level Two </t>
+  </si>
+  <si>
+    <t>Function Exercise Solutions - Challenge Problem</t>
+  </si>
+  <si>
+    <t>Lambda Expressions, Map, and Filter Functions </t>
+  </si>
+  <si>
+    <t>Nested Statements and Scope </t>
+  </si>
+  <si>
+    <t>Methods and Functions Homework Overview</t>
+  </si>
+  <si>
+    <t>Methods and Functions Homework - Solutions</t>
+  </si>
+  <si>
+    <t>–Milestone Project - 1</t>
+  </si>
+  <si>
+    <t>Introduction to Warm Up Project Exercises </t>
+  </si>
+  <si>
+    <t>Displaying Information </t>
+  </si>
+  <si>
+    <t>Accepting User Input </t>
+  </si>
+  <si>
+    <t>Validating User Input </t>
+  </si>
+  <si>
+    <t>Simple User Interaction </t>
+  </si>
+  <si>
+    <t>First Python Milestone Project Overview </t>
+  </si>
+  <si>
+    <t>Milestone Project Help </t>
+  </si>
+  <si>
+    <t>Solution Overview for MileStone Project 1 - Part One </t>
+  </si>
+  <si>
+    <t>Solution Overview for MileStone Project 1 - Part Two </t>
+  </si>
+  <si>
+    <t>Advanced Project Solution Overview </t>
+  </si>
+  <si>
+    <t>–Object Oriented Programming</t>
+  </si>
+  <si>
+    <t>Object Oriented Programming - Introduction </t>
+  </si>
+  <si>
+    <t>Object Oriented Programming - Attributes and Class Keyword </t>
+  </si>
+  <si>
+    <t>Object Oriented Programming - Class Object Attributes and Methods </t>
+  </si>
+  <si>
+    <t>Object Oriented Programming - Inheritance and Polymorphism </t>
+  </si>
+  <si>
+    <t>Object Oriented Programming - Special (Magic/Dunder) Methods </t>
+  </si>
+  <si>
+    <t>Object Oriented Programming - Homework </t>
+  </si>
+  <si>
+    <t>Object Oriented Programming - Homework Solutions </t>
+  </si>
+  <si>
+    <t>Object Oriented Programming - Challenge Overview</t>
+  </si>
+  <si>
+    <t>Object Oriented Programming - Challenge Solution </t>
+  </si>
+  <si>
+    <t>–Modules and Packages</t>
+  </si>
+  <si>
+    <t>Pip Install and PyPi </t>
+  </si>
+  <si>
+    <t>Modules and Packages </t>
+  </si>
+  <si>
+    <t>__name__ and "__main__" </t>
+  </si>
+  <si>
+    <t>–Errors and Exceptions Handling</t>
+  </si>
+  <si>
+    <t>Errors and Exception Handling </t>
+  </si>
+  <si>
+    <t>Errors and Exceptions Homework </t>
+  </si>
+  <si>
+    <t>Errors and Exception Homework - Solutions </t>
+  </si>
+  <si>
+    <t>Update for Pylint Users</t>
+  </si>
+  <si>
+    <t>Pylint Overview </t>
+  </si>
+  <si>
+    <t>Running tests with the Unittest Library </t>
+  </si>
+  <si>
+    <t>–Milestone Project - 2</t>
+  </si>
+  <si>
+    <t>Introduction to Milestone Project 2 Section Warmup </t>
+  </si>
+  <si>
+    <t>Card Class </t>
+  </si>
+  <si>
+    <t>Deck Class </t>
+  </si>
+  <si>
+    <t>Player Class </t>
+  </si>
+  <si>
+    <t>Game Logic - Part One </t>
+  </si>
+  <si>
+    <t>Game Logic - Part Two </t>
+  </si>
+  <si>
+    <t>Game Logic - Part Three </t>
+  </si>
+  <si>
+    <t>Milestone Project 2 Overview </t>
+  </si>
+  <si>
+    <t>Solution Walkthrough - Card and Deck classes </t>
+  </si>
+  <si>
+    <t>Solution Walkthrough - Hand and Chip Classes </t>
+  </si>
+  <si>
+    <t>Solution Walkthrough - Functions for Game Play </t>
+  </si>
+  <si>
+    <t>Solutions Walkthrough - Final Gameplay Script </t>
+  </si>
+  <si>
+    <t>–Python Decorators</t>
+  </si>
+  <si>
+    <t>Decorators with Python Overview </t>
+  </si>
+  <si>
+    <t>Decorators Homework </t>
+  </si>
+  <si>
+    <t>–Python Generators</t>
+  </si>
+  <si>
+    <t>Generators with Python </t>
+  </si>
+  <si>
+    <t>Generators Homework Overview </t>
+  </si>
+  <si>
+    <t>Generators Homework Solutions </t>
+  </si>
+  <si>
+    <t>–Advanced Python Modules</t>
+  </si>
+  <si>
+    <t>Introduction to Advanced Python Modules </t>
+  </si>
+  <si>
+    <t>Python Collections Module </t>
+  </si>
+  <si>
+    <t>Opening and Reading Files and Folders (Python OS Module) </t>
+  </si>
+  <si>
+    <t>Python Datetime Module </t>
+  </si>
+  <si>
+    <t>Python Math and Random Modules </t>
+  </si>
+  <si>
+    <t>Python Debugger </t>
+  </si>
+  <si>
+    <t>Python Regular Expressions Part One </t>
+  </si>
+  <si>
+    <t>Python Regular Expressions Part Two </t>
+  </si>
+  <si>
+    <t>Python Regular Expressions Part Three </t>
+  </si>
+  <si>
+    <t>Timing Your Python Code </t>
+  </si>
+  <si>
+    <t>Zipping and Unzipping files with Python </t>
+  </si>
+  <si>
+    <t>Advanced Python Module Puzzle - Overview </t>
+  </si>
+  <si>
+    <t>Advanced Python Module Puzzle - Solution </t>
+  </si>
+  <si>
+    <t>–Web Scraping with Python</t>
+  </si>
+  <si>
+    <t>Introduction to Web Scraping </t>
+  </si>
+  <si>
+    <t>Setting Up Web Scraping Libraries </t>
+  </si>
+  <si>
+    <t>Python Web Scraping - Grabbing a Title </t>
+  </si>
+  <si>
+    <t>Python Web Scraping - Grabbing a Class </t>
+  </si>
+  <si>
+    <t>Python Web Scraping - Grabbing an Image </t>
+  </si>
+  <si>
+    <t>Python Web Scraping - Book Examples Part One </t>
+  </si>
+  <si>
+    <t>Python Web Scraping - Book Examples Part Two</t>
+  </si>
+  <si>
+    <t>Python Web Scraping - Exercise Overview </t>
+  </si>
+  <si>
+    <t>Preview04:12</t>
+  </si>
+  <si>
+    <t>Python Web Scraping - Exercise Solutions </t>
+  </si>
+  <si>
+    <t>–Working with Images with Python</t>
+  </si>
+  <si>
+    <t>Introduction to Images with Python </t>
+  </si>
+  <si>
+    <t>Working with Images with Python </t>
+  </si>
+  <si>
+    <t>Python Image Exercises - Overview </t>
+  </si>
+  <si>
+    <t>Python Image Exercises - Solution </t>
+  </si>
+  <si>
+    <t>–Working with PDFs and Spreadsheet CSV Files</t>
+  </si>
+  <si>
+    <t>Introduction to PDFs and Spreadsheets with Python </t>
+  </si>
+  <si>
+    <t>Working with CSV Files in Python </t>
+  </si>
+  <si>
+    <t>Working with PDF Files in Python </t>
+  </si>
+  <si>
+    <t>PDFs and Spreadsheets Python Puzzle Exercise </t>
+  </si>
+  <si>
+    <t>PDFs and Spreadsheets Python Puzzle Exercise - Solutions </t>
+  </si>
+  <si>
+    <t>–Emails with Python</t>
+  </si>
+  <si>
+    <t>Introduction to Emails with Python </t>
+  </si>
+  <si>
+    <t>Sending Emails with Python </t>
+  </si>
+  <si>
+    <t>Receiving Emails with Python </t>
+  </si>
+  <si>
+    <t>–Final Capstone Python Project</t>
+  </si>
+  <si>
+    <t>Final Capstone Project </t>
+  </si>
+  <si>
+    <t>–Advanced Python Objects and Data Structures</t>
+  </si>
+  <si>
+    <t>Advanced Numbers </t>
+  </si>
+  <si>
+    <t>Advanced Strings </t>
+  </si>
+  <si>
+    <t>Advanced Sets </t>
+  </si>
+  <si>
+    <t>Advanced Dictionaries </t>
+  </si>
+  <si>
+    <t>Advanced Lists </t>
+  </si>
+  <si>
+    <t>Advanced Python Objects Assessment Test </t>
+  </si>
+  <si>
+    <t>Advanced Python Objects Test - Solutions </t>
+  </si>
+  <si>
+    <t>–Bonus Material - Introduction to GUIs</t>
+  </si>
+  <si>
+    <t>Introduction to GUIs </t>
+  </si>
+  <si>
+    <t>Quick note about ipywidgets</t>
+  </si>
+  <si>
+    <t>Interact Functionality with GUIs </t>
+  </si>
+  <si>
+    <t>GUI Widget Basics </t>
+  </si>
+  <si>
+    <t>List of Possible Widgets </t>
+  </si>
+  <si>
+    <t>Widget Styling and Layouts </t>
+  </si>
+  <si>
+    <t>Example of what a Widget can do! </t>
+  </si>
+  <si>
+    <t>–BONUS SECTION: THANK YOU!</t>
+  </si>
+  <si>
+    <t>BONUS LECTURE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -349,6 +970,38 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF505763"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF505763"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF686F7A"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF007791"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -371,14 +1024,47 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="21" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="46" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -680,7 +1366,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
+    <sheetView topLeftCell="A75" workbookViewId="0">
       <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
@@ -1248,13 +1934,2244 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A406"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="60.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="12">
+        <v>39264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>0.90365740740740741</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>0.80208333333333337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>3.0555555555555555E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6">
+        <v>0.22083333333333333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>0.10625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>1.6486111111111112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6">
+        <v>0.34375</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6">
+        <v>0.74305555555555547</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
+        <v>9.8611111111111108E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
+        <v>0.1173611111111111</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
+        <v>8.4976851851851845E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6">
+        <v>0.16805555555555554</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6">
+        <v>9.7222222222222224E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="6">
+        <v>0.32916666666666666</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6">
+        <v>0.2986111111111111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6">
+        <v>0.35347222222222219</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="6">
+        <v>0.39374999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="6">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="6">
+        <v>0.49305555555555558</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="6">
+        <v>2.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="6">
+        <v>0.48749999999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="6">
+        <v>8.3333333333333332E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" s="6">
+        <v>0.44375000000000003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76" s="6">
+        <v>9.0277777777777787E-3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80" s="6">
+        <v>0.20069444444444443</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81" s="5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84" s="6">
+        <v>0.1173611111111111</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88" s="6">
+        <v>0.12986111111111112</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92" s="6">
+        <v>0.7402777777777777</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96" s="6">
+        <v>1.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98" s="6">
+        <v>0.28333333333333333</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100" s="6">
+        <v>0.40763888888888888</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102" s="4">
+        <v>0.38055555555555554</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104" s="6">
+        <v>0.14305555555555557</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106" s="6">
+        <v>0.23750000000000002</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108" s="11" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110" s="10">
+        <v>5.229166666666666E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112" s="6">
+        <v>0.37916666666666665</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113" s="7" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116" s="6">
+        <v>0.44097222222222227</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118" s="6">
+        <v>0.67222222222222217</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120" s="6">
+        <v>0.47638888888888892</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122" s="6">
+        <v>0.10208333333333335</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124" s="6">
+        <v>0.30486111111111108</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126" s="10">
+        <v>0.12078703703703704</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128" s="6">
+        <v>0.29444444444444445</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130" s="6">
+        <v>0.13125000000000001</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132" s="6">
+        <v>0.23750000000000002</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134" s="6">
+        <v>0.46180555555555558</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136" s="6">
+        <v>0.5131944444444444</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138" s="6">
+        <v>0.37152777777777773</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140" s="6">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142" s="6">
+        <v>4.5833333333333337E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145" s="5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155" s="5" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157" s="5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A159" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A160" s="6">
+        <v>0.50069444444444444</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A161" s="5" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A162" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A163" s="5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A164" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A165" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A166" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A167" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A168" s="6">
+        <v>0.20486111111111113</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A169" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A170" s="6">
+        <v>0.41875000000000001</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A171" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A172" s="6">
+        <v>0.30555555555555552</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A173" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A174" s="6">
+        <v>0.47569444444444442</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A175" s="5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A176" s="6">
+        <v>0.55277777777777781</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A177" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A178" s="6">
+        <v>0.56666666666666665</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A179" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A180" s="6">
+        <v>0.66805555555555562</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A181" s="5" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A182" s="6">
+        <v>0.24930555555555556</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A183" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A184" s="6">
+        <v>0.7993055555555556</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A185" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A186" s="10">
+        <v>7.525462962962963E-2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A187" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A188" s="6">
+        <v>0.15763888888888888</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A189" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A190" s="6">
+        <v>0.22708333333333333</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A191" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A192" s="6">
+        <v>0.4291666666666667</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A193" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A194" s="6">
+        <v>0.77708333333333324</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A195" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A196" s="6">
+        <v>0.59722222222222221</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A197" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A198" s="6">
+        <v>0.65138888888888891</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A199" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A200" s="6">
+        <v>0.12430555555555556</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A201" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A202" s="6">
+        <v>0.66736111111111107</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A203" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A204" s="6">
+        <v>0.5444444444444444</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A205" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A206" s="6">
+        <v>0.33958333333333335</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A207" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A208" s="10">
+        <v>5.6122685185185185E-2</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A209" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A210" s="6">
+        <v>0.20277777777777781</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A211" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A212" s="6">
+        <v>0.59652777777777777</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A213" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A214" s="6">
+        <v>0.72083333333333333</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A215" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A216" s="6">
+        <v>0.69791666666666663</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A217" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A218" s="6">
+        <v>0.29236111111111113</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A219" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A220" s="6">
+        <v>0.12986111111111112</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A221" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A222" s="6">
+        <v>0.28541666666666665</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A223" s="5" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A224" s="6">
+        <v>0.21805555555555556</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A225" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A226" s="6">
+        <v>0.22361111111111109</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A227" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A228" s="9">
+        <v>1.2152777777777779</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A229" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A230" s="6">
+        <v>0.32361111111111113</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A231" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A232" s="6">
+        <v>0.48541666666666666</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A233" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A234" s="6">
+        <v>0.40625</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A235" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A236" s="9">
+        <v>1.8986111111111112</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A237" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A238" s="6">
+        <v>0.72152777777777777</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A239" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A240" s="6">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A241" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A242" s="6">
+        <v>0.21944444444444444</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A243" s="5" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A244" s="6">
+        <v>1.3888888888888888E-2</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A245" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A246" s="6">
+        <v>0.48333333333333334</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A247" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A248" s="6">
+        <v>0.3979166666666667</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A249" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A250" s="10">
+        <v>8.9004629629629628E-2</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A251" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A252" s="6">
+        <v>0.15902777777777777</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A253" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A254" s="6">
+        <v>0.49791666666666662</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A255" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A256" s="6">
+        <v>0.66111111111111109</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A257" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A258" s="6">
+        <v>0.46111111111111108</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A259" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A260" s="6">
+        <v>0.23819444444444446</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A261" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A262" s="6">
+        <v>0.33611111111111108</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A263" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A264" s="6">
+        <v>0.68888888888888899</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A265" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A266" s="6">
+        <v>0.35902777777777778</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A267" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A268" s="6">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A269" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A270" s="6">
+        <v>0.59861111111111109</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A271" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A272" s="6">
+        <v>0.38263888888888892</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A273" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A274" s="6">
+        <v>0.50763888888888886</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A275" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A276" s="4">
+        <v>0.97569444444444453</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A277" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A278" s="6">
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A279" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A280" s="6">
+        <v>8.6805555555555566E-2</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A281" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A282" s="4">
+        <v>0.72013888888888899</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A283" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A284" s="6">
+        <v>0.54583333333333328</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A285" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A286" s="6">
+        <v>6.9444444444444434E-2</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A287" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A288" s="6">
+        <v>0.10486111111111111</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A289" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A290" s="10">
+        <v>9.9085648148148145E-2</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A291" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A292" s="6">
+        <v>3.8194444444444441E-2</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A293" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A294" s="6">
+        <v>0.5395833333333333</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A295" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A296" s="6">
+        <v>0.8208333333333333</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A297" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A298" s="6">
+        <v>0.47361111111111115</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A299" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A300" s="6">
+        <v>0.65555555555555556</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A301" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A302" s="6">
+        <v>0.28541666666666665</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A303" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A304" s="6">
+        <v>0.47986111111111113</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A305" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A306" s="6">
+        <v>0.60555555555555551</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A307" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A308" s="6">
+        <v>0.58611111111111114</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A309" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A310" s="6">
+        <v>0.52222222222222225</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A311" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A312" s="6">
+        <v>0.43472222222222223</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A313" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A314" s="6">
+        <v>7.5694444444444439E-2</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A315" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A316" s="6">
+        <v>0.42777777777777781</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A317" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A318" s="10">
+        <v>6.9386574074074073E-2</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A319" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A320" s="6">
+        <v>0.65277777777777779</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A321" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A322" s="6">
+        <v>0.28958333333333336</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A323" s="3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A324" s="6">
+        <v>0.42569444444444443</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A325" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A326" s="6">
+        <v>0.3444444444444445</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A327" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A328" s="6">
+        <v>0.64583333333333337</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A329" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A330" s="6">
+        <v>0.4069444444444445</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A331" s="5" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A332" s="6">
+        <v>0.55625000000000002</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A333" s="7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A334" s="8" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A335" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A336" s="6">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A337" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A338" s="9">
+        <v>1.0055555555555555</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A339" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A340" s="6">
+        <v>2.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A341" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A342" s="6">
+        <v>0.75347222222222221</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A343" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A344" s="6">
+        <v>8.0555555555555561E-2</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A345" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A346" s="6">
+        <v>0.14652777777777778</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A347" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A348" s="9">
+        <v>1.8638888888888889</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A349" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A350" s="6">
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A351" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A352" s="6">
+        <v>0.81041666666666667</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A353" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A354" s="6">
+        <v>0.52569444444444446</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A355" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A356" s="6">
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A357" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A358" s="6">
+        <v>0.41319444444444442</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A359" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A360" s="9">
+        <v>1.1666666666666667</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A361" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A362" s="6">
+        <v>6.3194444444444442E-2</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A363" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A364" s="6">
+        <v>0.5708333333333333</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A365" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A366" s="6">
+        <v>0.53263888888888888</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A367" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A368" s="4">
+        <v>0.13541666666666666</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A369" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A370" s="6">
+        <v>0.13541666666666666</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A371" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A372" s="9">
+        <v>1.6986111111111111</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A373" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A374" s="6">
+        <v>0.18958333333333333</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A375" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A376" s="6">
+        <v>0.35416666666666669</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A377" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A378" s="6">
+        <v>0.47569444444444442</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A379" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A380" s="6">
+        <v>0.20972222222222223</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A381" s="3" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A382" s="6">
+        <v>0.34722222222222227</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A383" s="3" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A384" s="6">
+        <v>7.3611111111111113E-2</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A385" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A386" s="6">
+        <v>4.8611111111111112E-2</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A387" s="3" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A388" s="9">
+        <v>1.8854166666666667</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A389" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A390" s="6">
+        <v>3.6111111111111115E-2</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A391" s="5" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A392" s="6">
+        <v>5.5555555555555558E-3</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A393" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A394" s="6">
+        <v>0.65277777777777779</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A395" s="3" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A396" s="6">
+        <v>0.34166666666666662</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A397" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A398" s="6">
+        <v>0.26319444444444445</v>
+      </c>
+    </row>
+    <row r="399" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A399" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A400" s="6">
+        <v>0.34027777777777773</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A401" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A402" s="6">
+        <v>0.24513888888888888</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A403" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A404" s="4">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A405" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A406" s="6">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" display="javascript:void(0)"/>
+    <hyperlink ref="A4" r:id="rId2" display="javascript:void(0)"/>
+    <hyperlink ref="A5" r:id="rId3" display="javascript:void(0)"/>
+    <hyperlink ref="A8" r:id="rId4" display="javascript:void(0)"/>
+    <hyperlink ref="A9" r:id="rId5" display="javascript:void(0)"/>
+    <hyperlink ref="A11" r:id="rId6" display="javascript:void(0)"/>
+    <hyperlink ref="A13" r:id="rId7" display="javascript:void(0)"/>
+    <hyperlink ref="A15" r:id="rId8" display="javascript:void(0)"/>
+    <hyperlink ref="A16" r:id="rId9" display="javascript:void(0)"/>
+    <hyperlink ref="A17" r:id="rId10" display="javascript:void(0)"/>
+    <hyperlink ref="A20" r:id="rId11" display="javascript:void(0)"/>
+    <hyperlink ref="A21" r:id="rId12" display="javascript:void(0)"/>
+    <hyperlink ref="A23" r:id="rId13" display="javascript:void(0)"/>
+    <hyperlink ref="A25" r:id="rId14" display="javascript:void(0)"/>
+    <hyperlink ref="A27" r:id="rId15" display="javascript:void(0)"/>
+    <hyperlink ref="A28" r:id="rId16" display="javascript:void(0)"/>
+    <hyperlink ref="A29" r:id="rId17" display="javascript:void(0)"/>
+    <hyperlink ref="A32" r:id="rId18" display="javascript:void(0)"/>
+    <hyperlink ref="A35" r:id="rId19" display="javascript:void(0)"/>
+    <hyperlink ref="A37" r:id="rId20" display="javascript:void(0)"/>
+    <hyperlink ref="A39" r:id="rId21" display="javascript:void(0)"/>
+    <hyperlink ref="A41" r:id="rId22" display="javascript:void(0)"/>
+    <hyperlink ref="A45" r:id="rId23" display="javascript:void(0)"/>
+    <hyperlink ref="A51" r:id="rId24" display="javascript:void(0)"/>
+    <hyperlink ref="A53" r:id="rId25" display="javascript:void(0)"/>
+    <hyperlink ref="A57" r:id="rId26" display="javascript:void(0)"/>
+    <hyperlink ref="A59" r:id="rId27" display="javascript:void(0)"/>
+    <hyperlink ref="A63" r:id="rId28" display="javascript:void(0)"/>
+    <hyperlink ref="A67" r:id="rId29" display="javascript:void(0)"/>
+    <hyperlink ref="A71" r:id="rId30" display="javascript:void(0)"/>
+    <hyperlink ref="A75" r:id="rId31" display="javascript:void(0)"/>
+    <hyperlink ref="A79" r:id="rId32" display="javascript:void(0)"/>
+    <hyperlink ref="A83" r:id="rId33" display="javascript:void(0)"/>
+    <hyperlink ref="A87" r:id="rId34" display="javascript:void(0)"/>
+    <hyperlink ref="A91" r:id="rId35" display="javascript:void(0)"/>
+    <hyperlink ref="A95" r:id="rId36" display="javascript:void(0)"/>
+    <hyperlink ref="A97" r:id="rId37" display="javascript:void(0)"/>
+    <hyperlink ref="A99" r:id="rId38" display="javascript:void(0)"/>
+    <hyperlink ref="A101" r:id="rId39" display="javascript:void(0)"/>
+    <hyperlink ref="A102" r:id="rId40" display="javascript:void(0)"/>
+    <hyperlink ref="A103" r:id="rId41" display="javascript:void(0)"/>
+    <hyperlink ref="A105" r:id="rId42" display="javascript:void(0)"/>
+    <hyperlink ref="A107" r:id="rId43" display="javascript:void(0)"/>
+    <hyperlink ref="A109" r:id="rId44" display="javascript:void(0)"/>
+    <hyperlink ref="A110" r:id="rId45" display="javascript:void(0)"/>
+    <hyperlink ref="A111" r:id="rId46" display="javascript:void(0)"/>
+    <hyperlink ref="A114" r:id="rId47" display="javascript:void(0)"/>
+    <hyperlink ref="A115" r:id="rId48" display="javascript:void(0)"/>
+    <hyperlink ref="A117" r:id="rId49" display="javascript:void(0)"/>
+    <hyperlink ref="A119" r:id="rId50" display="javascript:void(0)"/>
+    <hyperlink ref="A121" r:id="rId51" display="javascript:void(0)"/>
+    <hyperlink ref="A123" r:id="rId52" display="javascript:void(0)"/>
+    <hyperlink ref="A125" r:id="rId53" display="javascript:void(0)"/>
+    <hyperlink ref="A126" r:id="rId54" display="javascript:void(0)"/>
+    <hyperlink ref="A127" r:id="rId55" display="javascript:void(0)"/>
+    <hyperlink ref="A129" r:id="rId56" display="javascript:void(0)"/>
+    <hyperlink ref="A131" r:id="rId57" display="javascript:void(0)"/>
+    <hyperlink ref="A133" r:id="rId58" display="javascript:void(0)"/>
+    <hyperlink ref="A135" r:id="rId59" display="javascript:void(0)"/>
+    <hyperlink ref="A137" r:id="rId60" display="javascript:void(0)"/>
+    <hyperlink ref="A139" r:id="rId61" display="javascript:void(0)"/>
+    <hyperlink ref="A141" r:id="rId62" display="javascript:void(0)"/>
+    <hyperlink ref="A143" r:id="rId63" display="javascript:void(0)"/>
+    <hyperlink ref="A159" r:id="rId64" display="javascript:void(0)"/>
+    <hyperlink ref="A167" r:id="rId65" display="javascript:void(0)"/>
+    <hyperlink ref="A169" r:id="rId66" display="javascript:void(0)"/>
+    <hyperlink ref="A171" r:id="rId67" display="javascript:void(0)"/>
+    <hyperlink ref="A173" r:id="rId68" display="javascript:void(0)"/>
+    <hyperlink ref="A177" r:id="rId69" display="javascript:void(0)"/>
+    <hyperlink ref="A179" r:id="rId70" display="javascript:void(0)"/>
+    <hyperlink ref="A185" r:id="rId71" display="javascript:void(0)"/>
+    <hyperlink ref="A186" r:id="rId72" display="javascript:void(0)"/>
+    <hyperlink ref="A187" r:id="rId73" display="javascript:void(0)"/>
+    <hyperlink ref="A189" r:id="rId74" display="javascript:void(0)"/>
+    <hyperlink ref="A191" r:id="rId75" display="javascript:void(0)"/>
+    <hyperlink ref="A193" r:id="rId76" display="javascript:void(0)"/>
+    <hyperlink ref="A195" r:id="rId77" display="javascript:void(0)"/>
+    <hyperlink ref="A197" r:id="rId78" display="javascript:void(0)"/>
+    <hyperlink ref="A199" r:id="rId79" display="javascript:void(0)"/>
+    <hyperlink ref="A201" r:id="rId80" display="javascript:void(0)"/>
+    <hyperlink ref="A203" r:id="rId81" display="javascript:void(0)"/>
+    <hyperlink ref="A205" r:id="rId82" display="javascript:void(0)"/>
+    <hyperlink ref="A207" r:id="rId83" display="javascript:void(0)"/>
+    <hyperlink ref="A208" r:id="rId84" display="javascript:void(0)"/>
+    <hyperlink ref="A209" r:id="rId85" display="javascript:void(0)"/>
+    <hyperlink ref="A211" r:id="rId86" display="javascript:void(0)"/>
+    <hyperlink ref="A213" r:id="rId87" display="javascript:void(0)"/>
+    <hyperlink ref="A215" r:id="rId88" display="javascript:void(0)"/>
+    <hyperlink ref="A217" r:id="rId89" display="javascript:void(0)"/>
+    <hyperlink ref="A219" r:id="rId90" display="javascript:void(0)"/>
+    <hyperlink ref="A221" r:id="rId91" display="javascript:void(0)"/>
+    <hyperlink ref="A225" r:id="rId92" display="javascript:void(0)"/>
+    <hyperlink ref="A227" r:id="rId93" display="javascript:void(0)"/>
+    <hyperlink ref="A228" r:id="rId94" display="javascript:void(0)"/>
+    <hyperlink ref="A229" r:id="rId95" display="javascript:void(0)"/>
+    <hyperlink ref="A231" r:id="rId96" display="javascript:void(0)"/>
+    <hyperlink ref="A233" r:id="rId97" display="javascript:void(0)"/>
+    <hyperlink ref="A235" r:id="rId98" display="javascript:void(0)"/>
+    <hyperlink ref="A236" r:id="rId99" display="javascript:void(0)"/>
+    <hyperlink ref="A237" r:id="rId100" display="javascript:void(0)"/>
+    <hyperlink ref="A239" r:id="rId101" display="javascript:void(0)"/>
+    <hyperlink ref="A241" r:id="rId102" display="javascript:void(0)"/>
+    <hyperlink ref="A245" r:id="rId103" display="javascript:void(0)"/>
+    <hyperlink ref="A247" r:id="rId104" display="javascript:void(0)"/>
+    <hyperlink ref="A249" r:id="rId105" display="javascript:void(0)"/>
+    <hyperlink ref="A250" r:id="rId106" display="javascript:void(0)"/>
+    <hyperlink ref="A251" r:id="rId107" display="javascript:void(0)"/>
+    <hyperlink ref="A253" r:id="rId108" display="javascript:void(0)"/>
+    <hyperlink ref="A255" r:id="rId109" display="javascript:void(0)"/>
+    <hyperlink ref="A257" r:id="rId110" display="javascript:void(0)"/>
+    <hyperlink ref="A259" r:id="rId111" display="javascript:void(0)"/>
+    <hyperlink ref="A261" r:id="rId112" display="javascript:void(0)"/>
+    <hyperlink ref="A263" r:id="rId113" display="javascript:void(0)"/>
+    <hyperlink ref="A265" r:id="rId114" display="javascript:void(0)"/>
+    <hyperlink ref="A267" r:id="rId115" display="javascript:void(0)"/>
+    <hyperlink ref="A269" r:id="rId116" display="javascript:void(0)"/>
+    <hyperlink ref="A271" r:id="rId117" display="javascript:void(0)"/>
+    <hyperlink ref="A273" r:id="rId118" display="javascript:void(0)"/>
+    <hyperlink ref="A275" r:id="rId119" display="javascript:void(0)"/>
+    <hyperlink ref="A276" r:id="rId120" display="javascript:void(0)"/>
+    <hyperlink ref="A277" r:id="rId121" display="javascript:void(0)"/>
+    <hyperlink ref="A279" r:id="rId122" display="javascript:void(0)"/>
+    <hyperlink ref="A281" r:id="rId123" display="javascript:void(0)"/>
+    <hyperlink ref="A282" r:id="rId124" display="javascript:void(0)"/>
+    <hyperlink ref="A283" r:id="rId125" display="javascript:void(0)"/>
+    <hyperlink ref="A285" r:id="rId126" display="javascript:void(0)"/>
+    <hyperlink ref="A287" r:id="rId127" display="javascript:void(0)"/>
+    <hyperlink ref="A289" r:id="rId128" display="javascript:void(0)"/>
+    <hyperlink ref="A290" r:id="rId129" display="javascript:void(0)"/>
+    <hyperlink ref="A291" r:id="rId130" display="javascript:void(0)"/>
+    <hyperlink ref="A293" r:id="rId131" display="javascript:void(0)"/>
+    <hyperlink ref="A295" r:id="rId132" display="javascript:void(0)"/>
+    <hyperlink ref="A297" r:id="rId133" display="javascript:void(0)"/>
+    <hyperlink ref="A299" r:id="rId134" display="javascript:void(0)"/>
+    <hyperlink ref="A301" r:id="rId135" display="javascript:void(0)"/>
+    <hyperlink ref="A303" r:id="rId136" display="javascript:void(0)"/>
+    <hyperlink ref="A305" r:id="rId137" display="javascript:void(0)"/>
+    <hyperlink ref="A307" r:id="rId138" display="javascript:void(0)"/>
+    <hyperlink ref="A309" r:id="rId139" display="javascript:void(0)"/>
+    <hyperlink ref="A311" r:id="rId140" display="javascript:void(0)"/>
+    <hyperlink ref="A313" r:id="rId141" display="javascript:void(0)"/>
+    <hyperlink ref="A315" r:id="rId142" display="javascript:void(0)"/>
+    <hyperlink ref="A317" r:id="rId143" display="javascript:void(0)"/>
+    <hyperlink ref="A318" r:id="rId144" display="javascript:void(0)"/>
+    <hyperlink ref="A319" r:id="rId145" display="javascript:void(0)"/>
+    <hyperlink ref="A321" r:id="rId146" display="javascript:void(0)"/>
+    <hyperlink ref="A323" r:id="rId147" display="javascript:void(0)"/>
+    <hyperlink ref="A325" r:id="rId148" display="javascript:void(0)"/>
+    <hyperlink ref="A327" r:id="rId149" display="javascript:void(0)"/>
+    <hyperlink ref="A329" r:id="rId150" display="javascript:void(0)"/>
+    <hyperlink ref="A334" r:id="rId151" display="javascript:void(0)"/>
+    <hyperlink ref="A335" r:id="rId152" display="javascript:void(0)"/>
+    <hyperlink ref="A337" r:id="rId153" display="javascript:void(0)"/>
+    <hyperlink ref="A338" r:id="rId154" display="javascript:void(0)"/>
+    <hyperlink ref="A339" r:id="rId155" display="javascript:void(0)"/>
+    <hyperlink ref="A341" r:id="rId156" display="javascript:void(0)"/>
+    <hyperlink ref="A343" r:id="rId157" display="javascript:void(0)"/>
+    <hyperlink ref="A345" r:id="rId158" display="javascript:void(0)"/>
+    <hyperlink ref="A347" r:id="rId159" display="javascript:void(0)"/>
+    <hyperlink ref="A348" r:id="rId160" display="javascript:void(0)"/>
+    <hyperlink ref="A349" r:id="rId161" display="javascript:void(0)"/>
+    <hyperlink ref="A351" r:id="rId162" display="javascript:void(0)"/>
+    <hyperlink ref="A353" r:id="rId163" display="javascript:void(0)"/>
+    <hyperlink ref="A355" r:id="rId164" display="javascript:void(0)"/>
+    <hyperlink ref="A357" r:id="rId165" display="javascript:void(0)"/>
+    <hyperlink ref="A359" r:id="rId166" display="javascript:void(0)"/>
+    <hyperlink ref="A360" r:id="rId167" display="javascript:void(0)"/>
+    <hyperlink ref="A361" r:id="rId168" display="javascript:void(0)"/>
+    <hyperlink ref="A363" r:id="rId169" display="javascript:void(0)"/>
+    <hyperlink ref="A365" r:id="rId170" display="javascript:void(0)"/>
+    <hyperlink ref="A367" r:id="rId171" display="javascript:void(0)"/>
+    <hyperlink ref="A368" r:id="rId172" display="javascript:void(0)"/>
+    <hyperlink ref="A369" r:id="rId173" display="javascript:void(0)"/>
+    <hyperlink ref="A371" r:id="rId174" display="javascript:void(0)"/>
+    <hyperlink ref="A372" r:id="rId175" display="javascript:void(0)"/>
+    <hyperlink ref="A373" r:id="rId176" display="javascript:void(0)"/>
+    <hyperlink ref="A375" r:id="rId177" display="javascript:void(0)"/>
+    <hyperlink ref="A377" r:id="rId178" display="javascript:void(0)"/>
+    <hyperlink ref="A379" r:id="rId179" display="javascript:void(0)"/>
+    <hyperlink ref="A381" r:id="rId180" display="javascript:void(0)"/>
+    <hyperlink ref="A383" r:id="rId181" display="javascript:void(0)"/>
+    <hyperlink ref="A385" r:id="rId182" display="javascript:void(0)"/>
+    <hyperlink ref="A387" r:id="rId183" display="javascript:void(0)"/>
+    <hyperlink ref="A388" r:id="rId184" display="javascript:void(0)"/>
+    <hyperlink ref="A389" r:id="rId185" display="javascript:void(0)"/>
+    <hyperlink ref="A393" r:id="rId186" display="javascript:void(0)"/>
+    <hyperlink ref="A395" r:id="rId187" display="javascript:void(0)"/>
+    <hyperlink ref="A397" r:id="rId188" display="javascript:void(0)"/>
+    <hyperlink ref="A399" r:id="rId189" display="javascript:void(0)"/>
+    <hyperlink ref="A401" r:id="rId190" display="javascript:void(0)"/>
+    <hyperlink ref="A403" r:id="rId191" display="javascript:void(0)"/>
+    <hyperlink ref="A404" r:id="rId192" display="javascript:void(0)"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId193"/>
 </worksheet>
 </file>
 

</xml_diff>